<commit_message>
add 2019-11-19 files and add diff en/  zh/ python code
</commit_message>
<xml_diff>
--- a/data/istio 中文翻译统计表.xlsx
+++ b/data/istio 中文翻译统计表.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,102 +387,102 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>huntsman-li</t>
+          <t>ilylia</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11209</v>
+        <v>15015</v>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ilylia</t>
+          <t>huntsman-li</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6931</v>
+        <v>11209</v>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>yuxiaobo96</t>
+          <t>JasonRD</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2875</v>
+        <v>5795</v>
       </c>
       <c r="C4" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>idefav</t>
+          <t>dk-lockdown</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2423</v>
+        <v>3434</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>niceforbear</t>
+          <t>yuer1727</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2282</v>
+        <v>3413</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JasonRD</t>
+          <t>luxious</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2220</v>
+        <v>3278</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>gorda</t>
+          <t>yuxiaobo96</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2170</v>
+        <v>3182</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>luxious</t>
+          <t>vivian99-wu</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1943</v>
+        <v>3076</v>
       </c>
       <c r="C9" t="n">
         <v>3</v>
@@ -491,50 +491,50 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GuangmingLuo</t>
+          <t>cocotyty</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1861</v>
+        <v>2765</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>zqzzq</t>
+          <t>ExBs2724</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1858</v>
+        <v>2636</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>malphi</t>
+          <t>tanjunchen</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1606</v>
+        <v>2520</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>yuer1727</t>
+          <t>idefav</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1570</v>
+        <v>2423</v>
       </c>
       <c r="C13" t="n">
         <v>2</v>
@@ -543,219 +543,219 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>sirius1024</t>
+          <t>niceforbear</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1497</v>
+        <v>2282</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>wangzewang</t>
+          <t>gorda</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1412</v>
+        <v>2170</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>rootsongjc</t>
+          <t>Lovnx</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1272</v>
+        <v>1995</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>dk-lockdown</t>
+          <t>GuangmingLuo</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1224</v>
+        <v>1861</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>cocotyty</t>
+          <t>zqzzq</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1075</v>
+        <v>1858</v>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>wenhuwang</t>
+          <t>malphi</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>974</v>
+        <v>1606</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>homilly</t>
+          <t>sirius1024</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>880</v>
+        <v>1497</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>tolbkni</t>
+          <t>wangzewang</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>877</v>
+        <v>1412</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>jakeslee</t>
+          <t>rootsongjc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>831</v>
+        <v>1272</v>
       </c>
       <c r="C22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>gaohuag</t>
+          <t>WisWang</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>726</v>
+        <v>1185</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>zyt312074545</t>
+          <t>arunfung</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>719</v>
+        <v>1095</v>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>csdnshyang</t>
+          <t>JHDST</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>628</v>
+        <v>996</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>yuxiaoba</t>
+          <t>wenhuwang</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>513</v>
+        <v>974</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>JHDST</t>
+          <t>homilly</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>508</v>
+        <v>880</v>
       </c>
       <c r="C27" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>arunfung</t>
+          <t>tolbkni</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>465</v>
+        <v>877</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>WisWang</t>
+          <t>jakeslee</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>416</v>
+        <v>831</v>
       </c>
       <c r="C29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>shicheng0829</t>
+          <t>gaohuag</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>381</v>
+        <v>726</v>
       </c>
       <c r="C30" t="n">
         <v>1</v>
@@ -764,63 +764,63 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>zzzhy</t>
+          <t>zyt312074545</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>362</v>
+        <v>719</v>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>JuwanXu</t>
+          <t>csdnshyang</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>319</v>
+        <v>628</v>
       </c>
       <c r="C32" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lovnx</t>
+          <t>yuxiaoba</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>302</v>
+        <v>513</v>
       </c>
       <c r="C33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AsCat</t>
+          <t>zxh326</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>228</v>
+        <v>468</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ExBs2724</t>
+          <t>mrshengzyzy</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>197</v>
+        <v>456</v>
       </c>
       <c r="C35" t="n">
         <v>3</v>
@@ -829,50 +829,50 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>lilinji</t>
+          <t>JuwanXu</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>189</v>
+        <v>395</v>
       </c>
       <c r="C36" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>zxh326</t>
+          <t>shicheng0829</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>181</v>
+        <v>381</v>
       </c>
       <c r="C37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>qunqiang</t>
+          <t>zzzhy</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>179</v>
+        <v>362</v>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>mrshengzyzy</t>
+          <t>AsCat</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="C39" t="n">
         <v>1</v>
@@ -881,50 +881,50 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>sunny0826</t>
+          <t>TomatoAres</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>dotw</t>
+          <t>lilinji</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>kylesliu</t>
+          <t>qunqiang</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="C42" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GanymedeNil</t>
+          <t>sunny0826</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="C43" t="n">
         <v>1</v>
@@ -933,24 +933,24 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>innerpeacez</t>
+          <t>lengrongfu</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>76</v>
+        <v>147</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Luluda</t>
+          <t>wuti1609</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>41</v>
+        <v>144</v>
       </c>
       <c r="C45" t="n">
         <v>1</v>
@@ -959,37 +959,37 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>vflong</t>
+          <t>dotw</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="C46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5idu</t>
+          <t>kylesliu</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>TomatoAres</t>
+          <t>GanymedeNil</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="C48" t="n">
         <v>1</v>
@@ -998,13 +998,78 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>innerpeacez</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>76</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Luluda</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>41</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>vflong</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>37</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>5idu</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>32</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>koonchen</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>22</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>sniperking1234</t>
         </is>
       </c>
-      <c r="B49" t="n">
+      <c r="B54" t="n">
         <v>10</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1019,7 +1084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,50 +1112,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>zyt312074545</t>
+          <t>tanjunchen</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>375</v>
+        <v>13506</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>idefav</t>
+          <t>hwdef</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>208</v>
+        <v>1538</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gorda</t>
+          <t>ExBs2724</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>195</v>
+        <v>588</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JasonRD</t>
+          <t>vivian99-wu</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>52</v>
+        <v>506</v>
       </c>
       <c r="C5" t="n">
         <v>3</v>
@@ -1099,13 +1164,117 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>zyt312074545</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>375</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>JasonRD</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>257</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ilylia</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>222</v>
+      </c>
+      <c r="C8" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lovnx</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>211</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>idefav</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>208</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WisWang</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>206</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>gorda</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>195</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>dk-lockdown</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>125</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>rootsongjc</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B14" t="n">
         <v>24</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C14" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>